<commit_message>
Commits analyzer.py and adds the analyzeNetIncome method from analyzer.py to main
</commit_message>
<xml_diff>
--- a/net_income_new.xlsx
+++ b/net_income_new.xlsx
@@ -1,50 +1,108 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cummi\Desktop\webscrap\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20863A2-D5E8-4E8C-AACC-30FA66DA2F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>AGR</t>
+  </si>
+  <si>
+    <t>goog</t>
+  </si>
+  <si>
+    <t>pltr</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -86,95 +144,35 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -498,114 +496,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="15.28515625" bestFit="1" customWidth="1" min="2" max="5"/>
-    <col width="12.28515625" customWidth="1" min="6" max="6"/>
+    <col min="2" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ticker</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="F1" s="5" t="inlineStr">
-        <is>
-          <t>G1</t>
-        </is>
-      </c>
-      <c r="G1" s="5" t="inlineStr">
-        <is>
-          <t>G2</t>
-        </is>
-      </c>
-      <c r="H1" s="5" t="inlineStr">
-        <is>
-          <t>G3</t>
-        </is>
-      </c>
-      <c r="I1" s="5" t="inlineStr">
-        <is>
-          <t>AGR</t>
-        </is>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>goog</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2">
         <v>59972000</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>76033000</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>40269000</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="2">
         <v>34343000</v>
       </c>
       <c r="F2" s="3">
-        <f>((D2+ E2)/E2)*100</f>
-        <v/>
+        <f>((D2- E2)/E2)*100</f>
+        <v>17.25533587630667</v>
+      </c>
+      <c r="G2">
+        <f>((C2- D2)/D2)*100</f>
+        <v>88.812734361419459</v>
+      </c>
+      <c r="H2">
+        <f>((B2- C2)/C2)*100</f>
+        <v>-21.123722594136758</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(F2:H2)</f>
+        <v>28.314782547863121</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>pltr</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="n">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
         <v>-373705</v>
       </c>
-      <c r="C3" s="6" t="n">
+      <c r="C3" s="4">
         <v>-520379</v>
       </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="4">
         <v>-1166391</v>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="4">
         <v>-579646</v>
       </c>
       <c r="F3" s="3">
-        <f>((D3+ E3)/E3)*100</f>
-        <v/>
+        <f>((D3- E3)/E3)*100</f>
+        <v>101.22471301449505</v>
+      </c>
+      <c r="G3">
+        <f>((C3- D3)/D3)*100</f>
+        <v>-55.385543955671814</v>
+      </c>
+      <c r="H3">
+        <f>((B3- C3)/C3)*100</f>
+        <v>-28.185995207339264</v>
+      </c>
+      <c r="I3" s="3">
+        <f>AVERAGE(F3:H3)</f>
+        <v>5.8843912838279913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>